<commit_message>
updated tabs tp include linking info
</commit_message>
<xml_diff>
--- a/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
+++ b/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/ingest-client/tests/importer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{62FC1068-9B36-074A-86D1-18D92E570FD1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C67EC50E-DB13-4541-8843-E2B697FC1E61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="5780" windowWidth="25560" windowHeight="14620" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="4700" windowWidth="32220" windowHeight="20480" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="project" sheetId="1" r:id="rId1"/>
-    <sheet name="contact" sheetId="3" r:id="rId2"/>
-    <sheet name="donor_organism" sheetId="4" r:id="rId3"/>
-    <sheet name="specimen_from_organism" sheetId="6" r:id="rId4"/>
-    <sheet name="cell_suspension" sheetId="7" r:id="rId5"/>
-    <sheet name="dissociation_process" sheetId="12" r:id="rId6"/>
-    <sheet name="enrichment_process" sheetId="13" r:id="rId7"/>
-    <sheet name="library_preparation_process" sheetId="14" r:id="rId8"/>
-    <sheet name="sequencing_process" sheetId="15" r:id="rId9"/>
-    <sheet name="protocol" sheetId="17" r:id="rId10"/>
-    <sheet name="sequence_file" sheetId="18" r:id="rId11"/>
+    <sheet name="Project" sheetId="1" r:id="rId1"/>
+    <sheet name="Contact" sheetId="3" r:id="rId2"/>
+    <sheet name="Donor" sheetId="4" r:id="rId3"/>
+    <sheet name="Specimen from organism" sheetId="6" r:id="rId4"/>
+    <sheet name="Cell suspension" sheetId="7" r:id="rId5"/>
+    <sheet name="Dissociation process" sheetId="12" r:id="rId6"/>
+    <sheet name="Enrichment process" sheetId="13" r:id="rId7"/>
+    <sheet name="Sequencing process" sheetId="15" r:id="rId8"/>
+    <sheet name="Library preparation process" sheetId="14" r:id="rId9"/>
+    <sheet name="Protocols" sheetId="17" r:id="rId10"/>
+    <sheet name="Sequence files" sheetId="18" r:id="rId11"/>
     <sheet name="schemas" sheetId="20" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="270">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -227,9 +227,6 @@
     <t>ID of the biomaterial to which this file relates</t>
   </si>
   <si>
-    <t>ID of the sequencing process to which this file relates</t>
-  </si>
-  <si>
     <t>read1</t>
   </si>
   <si>
@@ -435,12 +432,6 @@
   </si>
   <si>
     <t>second</t>
-  </si>
-  <si>
-    <t>dissociation_process_1||enrichment_process_1</t>
-  </si>
-  <si>
-    <t>library_preparation_process_1||sequencing_process_1</t>
   </si>
   <si>
     <t>10x_sequencing_protocol.pdf</t>
@@ -588,33 +579,6 @@
     <t xml:space="preserve">The type of protocol. </t>
   </si>
   <si>
-    <t>projects.project.project_core.project_title</t>
-  </si>
-  <si>
-    <t>projects.project.project_core.project_description</t>
-  </si>
-  <si>
-    <t>projects.project.project_core.project_shortname</t>
-  </si>
-  <si>
-    <t>projects.project.contact.contact_name</t>
-  </si>
-  <si>
-    <t>projects.project.contact.email</t>
-  </si>
-  <si>
-    <t>projects.project.contact.institution</t>
-  </si>
-  <si>
-    <t>projects.project.contact.laboratory</t>
-  </si>
-  <si>
-    <t>projects.project.contact.address</t>
-  </si>
-  <si>
-    <t>projects.project.contact.country</t>
-  </si>
-  <si>
     <t>biomaterials.donor_organism.biomaterial_core.biomaterial_id</t>
   </si>
   <si>
@@ -672,120 +636,9 @@
     <t>biomaterials.donor_organism.height_unit.ontology</t>
   </si>
   <si>
-    <t>biomaterials.donor_organism.is_living</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.biological_sex</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.weight</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.weight_unit.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.weight_unit.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.biomaterial_core.biomaterial_id</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.biomaterial_core.biomaterial_name</t>
-  </si>
-  <si>
     <t>biomaterials.specimen_from_organism.biomaterial_core.biomaterial_description</t>
   </si>
   <si>
-    <t>biomaterials.specimen_from_organism.biomaterial_core.ncbi_taxon_id</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.biomaterial_core.has_input_biomaterial</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.genus_species.text</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.organ.text</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.organ.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.state_of_specimen.ischemic_time</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.state_of_specimen.microscopic_description</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.state_of_specimen.ischemic_temperature</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.state_of_specimen.postmortem_interval</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.process_ids</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.biomaterial_core.biomaterial_id</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.biomaterial_core.biomaterial_name</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.biomaterial_core.biomaterial_description</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.biomaterial_core.ncbi_taxon_id</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.biomaterial_core.has_input_biomaterial</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.genus_species.text</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.total_estimated_cells</t>
-  </si>
-  <si>
-    <t>biomaterials.cell_suspension.process_ids</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.process_core.process_id</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.process_core.process_name</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.process_core.process_description</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.dissociation_method</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.nucleic_acid_source</t>
-  </si>
-  <si>
-    <t>rocesses.dissociation_process.protocol_ids</t>
-  </si>
-  <si>
-    <t>processes.enrichment_process.process_core.process_id</t>
-  </si>
-  <si>
-    <t>processes.enrichment_process.process_core.process_name</t>
-  </si>
-  <si>
-    <t>processes.enrichment_process.process_core.process_description</t>
-  </si>
-  <si>
-    <t>processes.enrichment_process.enrichment_method</t>
-  </si>
-  <si>
-    <t>processes.enrichment_process.markers</t>
-  </si>
-  <si>
-    <t>processes.dissociation_process.protocol_ids</t>
-  </si>
-  <si>
     <t>processes.library_preparation_process.process_core.process_id</t>
   </si>
   <si>
@@ -801,33 +654,6 @@
     <t>processes.library_preparation_process.cell_barcode.barcode_offset</t>
   </si>
   <si>
-    <t>processes.library_preparation_process.cell_barcode.barcode_length</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.input_nucleic_acid_molecule.text</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.input_nucleic_acid_molecule.ontology</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.library_construction_approach</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.end_bias</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.strand</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.umi_barcode.barcode_read</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.umi_barcode.barcode_offset</t>
-  </si>
-  <si>
-    <t>processes.library_preparation_process.umi_barcode.barcode_length</t>
-  </si>
-  <si>
     <t>processes.sequencing_process.process_core.process_id</t>
   </si>
   <si>
@@ -840,56 +666,215 @@
     <t>processes.sequencing_process.instrument_manufacturer_model.text</t>
   </si>
   <si>
-    <t>processes.sequencing_process.instrument_manufacturer_model.ontology</t>
-  </si>
-  <si>
-    <t>processes.sequencing_process.paired_ends</t>
-  </si>
-  <si>
-    <t>processes.sequencing_process.protocol_ids</t>
-  </si>
-  <si>
-    <t>files.sequence_file.file_core.file_name</t>
-  </si>
-  <si>
-    <t>files.sequence_file.file_core.file_format</t>
-  </si>
-  <si>
-    <t>files.sequence_file.read_index</t>
-  </si>
-  <si>
-    <t>files.sequence_file.lane_index</t>
-  </si>
-  <si>
-    <t>files.sequence_file.biomaterial_id</t>
-  </si>
-  <si>
-    <t>files.sequence_file.process_id</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_core.process_id</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_core.process_name</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_core.process_description</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_core.process_document</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_type.text</t>
-  </si>
-  <si>
-    <t>protocols.protocol.protocol_type.ontology</t>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/project/5.1.0/project</t>
+  </si>
+  <si>
+    <t>tab_config</t>
+  </si>
+  <si>
+    <t>https://ui.humancellatlas.org/template/human_10x.yaml</t>
+  </si>
+  <si>
+    <t>dissociation_process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.postmortem_interval</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.biomaterial_id</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.biomaterial_core.biomaterial_id</t>
+  </si>
+  <si>
+    <t>project.project_core.project_shortname</t>
+  </si>
+  <si>
+    <t>project.project_core.project_title</t>
+  </si>
+  <si>
+    <t>project.project_core.project_description</t>
+  </si>
+  <si>
+    <t>project.contact.contact_name</t>
+  </si>
+  <si>
+    <t>project.contact.email</t>
+  </si>
+  <si>
+    <t>project.contact.institution</t>
+  </si>
+  <si>
+    <t>project.contact.laboratory</t>
+  </si>
+  <si>
+    <t>project.contact.address</t>
+  </si>
+  <si>
+    <t>project.contact.country</t>
+  </si>
+  <si>
+    <t>donor_organism.is_living</t>
+  </si>
+  <si>
+    <t>donor_organism.biological_sex</t>
+  </si>
+  <si>
+    <t>donor_organism.weight</t>
+  </si>
+  <si>
+    <t>donor_organism.weight_unit.text</t>
+  </si>
+  <si>
+    <t>donor_organism.weight_unit.ontology</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.genus_species.text</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ.text</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ.ontology</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.ischemic_temperature</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.ischemic_time</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.microscopic_description</t>
+  </si>
+  <si>
+    <t>enrichment_process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.biomaterial_name</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.biomaterial_description</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.ncbi_taxon_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.genus_species.text</t>
+  </si>
+  <si>
+    <t>cell_suspension.total_estimated_cells</t>
+  </si>
+  <si>
+    <t>dissociation_process.process_core.process_name</t>
+  </si>
+  <si>
+    <t>dissociation_process.process_core.process_description</t>
+  </si>
+  <si>
+    <t>dissociation_process.dissociation_method</t>
+  </si>
+  <si>
+    <t>dissociation_process.nucleic_acid_source</t>
+  </si>
+  <si>
+    <t>enrichment_process.process_core.process_name</t>
+  </si>
+  <si>
+    <t>enrichment_process.process_core.process_description</t>
+  </si>
+  <si>
+    <t>enrichment_process.enrichment_method</t>
+  </si>
+  <si>
+    <t>enrichment_process.markers</t>
+  </si>
+  <si>
+    <t>library_preparation_process.cell_barcode.barcode_length</t>
+  </si>
+  <si>
+    <t>library_preparation_process.input_nucleic_acid_molecule.text</t>
+  </si>
+  <si>
+    <t>library_preparation_process.input_nucleic_acid_molecule.ontology</t>
+  </si>
+  <si>
+    <t>library_preparation_process.library_construction_approach</t>
+  </si>
+  <si>
+    <t>library_preparation_process.end_bias</t>
+  </si>
+  <si>
+    <t>library_preparation_process.strand</t>
+  </si>
+  <si>
+    <t>library_preparation_process.umi_barcode.barcode_read</t>
+  </si>
+  <si>
+    <t>library_preparation_process.umi_barcode.barcode_offset</t>
+  </si>
+  <si>
+    <t>library_preparation_process.umi_barcode.barcode_length</t>
+  </si>
+  <si>
+    <t>sequencing_process.instrument_manufacturer_model.ontology</t>
+  </si>
+  <si>
+    <t>sequencing_process.paired_ends</t>
+  </si>
+  <si>
+    <t>protocol.protocol_type.ontology</t>
+  </si>
+  <si>
+    <t>protocol.protocol_type.text</t>
+  </si>
+  <si>
+    <t>protocol.protocol_core.process_document</t>
+  </si>
+  <si>
+    <t>protocol.protocol_core.process_description</t>
+  </si>
+  <si>
+    <t>protocol.protocol_core.process_name</t>
+  </si>
+  <si>
+    <t>sequence_file.lane_index</t>
+  </si>
+  <si>
+    <t>sequence_file.read_index</t>
+  </si>
+  <si>
+    <t>sequence_file.file_core.file_format</t>
+  </si>
+  <si>
+    <t>sequence_file.file_core.file_name</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.biomaterial_core.biomaterial_name</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.biomaterial_core.ncbi_taxon_id</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.biomaterial_id</t>
+  </si>
+  <si>
+    <t>protocol.protocol_core.process_id</t>
+  </si>
+  <si>
+    <t>library_preparation_process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>sequencing_process.process_core.process_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -964,6 +949,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -988,7 +980,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -998,8 +990,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1079,8 +1072,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1089,6 +1084,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1391,27 +1387,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="4"/>
+    <col min="2" max="2" width="56" style="4" customWidth="1"/>
     <col min="3" max="3" width="68.83203125" style="4" customWidth="1"/>
     <col min="4" max="16384" width="34.5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -1432,13 +1428,13 @@
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1451,9 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1462,22 +1456,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -1494,45 +1488,45 @@
         <v>56</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>98</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>101</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1542,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,30 +1547,29 @@
     <col min="1" max="1" width="53" style="30" customWidth="1"/>
     <col min="2" max="2" width="32" style="30"/>
     <col min="3" max="3" width="49" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="32" style="30"/>
+    <col min="4" max="4" width="32" style="30"/>
+    <col min="5" max="5" width="42.6640625" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="32" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>263</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>57</v>
       </c>
@@ -1592,249 +1585,210 @@
       <c r="E2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="C4" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="30">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="30">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="30">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="30">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="30">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="30">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="30">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="30">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="30">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="30">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="30">
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="30">
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1845,13 +1799,39 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3EDEE3-1762-1549-AA46-291BDBEECBBC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="50.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A9495D8C-BE5B-5440-9FC2-EC4AF58F557A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1860,7 +1840,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1870,22 +1850,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="20" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -1918,199 +1898,199 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2123,88 +2103,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="30.33203125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="30.33203125" style="4"/>
+    <col min="1" max="1" width="77.5" style="4" customWidth="1"/>
+    <col min="2" max="3" width="30.33203125" style="4" customWidth="1"/>
+    <col min="4" max="20" width="30.33203125" style="4"/>
+    <col min="21" max="21" width="44.33203125" style="4" customWidth="1"/>
+    <col min="22" max="16384" width="30.33203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="11" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>203</v>
-      </c>
       <c r="T1" s="10" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="X1" s="10" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -2260,19 +2243,19 @@
         <v>26</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="D4" s="3">
         <v>9606</v>
@@ -2281,61 +2264,61 @@
         <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="X4" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="T4" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="U4" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2345,65 +2328,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" style="16"/>
+    <col min="1" max="1" width="75" style="16" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="51.5" style="16" customWidth="1"/>
-    <col min="4" max="8" width="32.1640625" style="16"/>
+    <col min="4" max="4" width="32.1640625" style="16"/>
+    <col min="5" max="5" width="69.6640625" style="16" customWidth="1"/>
+    <col min="6" max="8" width="32.1640625" style="16"/>
     <col min="9" max="9" width="48.6640625" style="16" customWidth="1"/>
     <col min="10" max="10" width="45.1640625" style="16" customWidth="1"/>
-    <col min="11" max="16384" width="32.1640625" style="16"/>
+    <col min="11" max="12" width="32.1640625" style="16"/>
+    <col min="13" max="13" width="77.1640625" style="16" customWidth="1"/>
+    <col min="14" max="16384" width="32.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>209</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>210</v>
+        <v>264</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>212</v>
+        <v>265</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -2440,50 +2430,56 @@
       <c r="M2" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:13" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="N2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:14" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="27" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="27">
         <v>9606</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J4" s="27">
         <v>7200</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L4" s="27">
         <v>19800</v>
       </c>
       <c r="M4" s="28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M6" s="23"/>
     </row>
   </sheetData>
@@ -2494,45 +2490,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="32.1640625" style="16"/>
+    <col min="1" max="1" width="51" style="16" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="16"/>
+    <col min="4" max="4" width="50.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="78.5" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="32.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -2558,19 +2561,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="D4" s="3">
         <v>9606</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>28</v>
@@ -2579,11 +2582,15 @@
         <v>39300000</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>133</v>
+        <v>122</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2597,27 +2604,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="30.1640625" style="4"/>
+    <col min="1" max="1" width="63.33203125" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="30.1640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -2643,19 +2651,19 @@
     <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2667,33 +2675,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="26.6640625" style="16"/>
+    <col min="1" max="3" width="26.6640625" style="16"/>
+    <col min="4" max="4" width="47.5" style="16" customWidth="1"/>
+    <col min="5" max="16384" width="26.6640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -2719,19 +2729,19 @@
     <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2740,167 +2750,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="8" width="29.33203125" style="16"/>
-    <col min="9" max="9" width="42.5" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="29.33203125" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="11" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="16">
-        <v>0</v>
-      </c>
-      <c r="F4" s="16">
-        <v>16</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="M4" s="16">
-        <v>16</v>
-      </c>
-      <c r="N4" s="16">
-        <v>10</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2913,25 +2767,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>256</v>
+        <v>198</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>262</v>
+        <v>254</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -2945,7 +2799,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>50</v>
@@ -2957,22 +2811,178 @@
     <row r="3" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="8" width="29.33203125" style="16"/>
+    <col min="9" max="9" width="42.5" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="29.33203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="11" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>121</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
+        <v>16</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="M4" s="16">
+        <v>16</v>
+      </c>
+      <c r="N4" s="16">
+        <v>10</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added checking of ontology field and schema info retrieval in template manager
</commit_message>
<xml_diff>
--- a/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
+++ b/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/ingest-client/tests/importer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/hca/latest/ingest-client/tests/importer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C67EC50E-DB13-4541-8843-E2B697FC1E61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CFB63BF-EE6F-7849-8A18-052D6C4DB154}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="4700" windowWidth="32220" windowHeight="20480" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="11260" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="268">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -579,66 +579,6 @@
     <t xml:space="preserve">The type of protocol. </t>
   </si>
   <si>
-    <t>biomaterials.donor_organism.biomaterial_core.biomaterial_id</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.biomaterial_core.biomaterial_name</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.biomaterial_core.biomaterial_description</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.biomaterial_core.ncbi_taxon_id</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.genus_species.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.death.cause_of_death</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.death.cold_perfused</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.medical_history.alcohol_history</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.medical_history.smoking_history</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.organism_age</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.organism_age_unit.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.organism_age_unit.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.development_stage.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.development_stage.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.disease.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.disease.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.height</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.height_unit.text</t>
-  </si>
-  <si>
-    <t>biomaterials.donor_organism.height_unit.ontology</t>
-  </si>
-  <si>
-    <t>biomaterials.specimen_from_organism.biomaterial_core.biomaterial_description</t>
-  </si>
-  <si>
     <t>processes.library_preparation_process.process_core.process_id</t>
   </si>
   <si>
@@ -699,24 +639,6 @@
     <t>project.project_core.project_description</t>
   </si>
   <si>
-    <t>project.contact.contact_name</t>
-  </si>
-  <si>
-    <t>project.contact.email</t>
-  </si>
-  <si>
-    <t>project.contact.institution</t>
-  </si>
-  <si>
-    <t>project.contact.laboratory</t>
-  </si>
-  <si>
-    <t>project.contact.address</t>
-  </si>
-  <si>
-    <t>project.contact.country</t>
-  </si>
-  <si>
     <t>donor_organism.is_living</t>
   </si>
   <si>
@@ -868,6 +790,78 @@
   </si>
   <si>
     <t>sequencing_process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>project.contributors.contact_name</t>
+  </si>
+  <si>
+    <t>project.contributors.email</t>
+  </si>
+  <si>
+    <t>project.contributors.institution</t>
+  </si>
+  <si>
+    <t>project.contributors.laboratory</t>
+  </si>
+  <si>
+    <t>project.contributors.address</t>
+  </si>
+  <si>
+    <t>project.contributors.country</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.biomaterial_name</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.biomaterial_description</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.ncbi_taxon_id</t>
+  </si>
+  <si>
+    <t>donor_organism.genus_species.text</t>
+  </si>
+  <si>
+    <t>donor_organism.death.cause_of_death</t>
+  </si>
+  <si>
+    <t>donor_organism.death.cold_perfused</t>
+  </si>
+  <si>
+    <t>donor_organism.medical_history.alcohol_history</t>
+  </si>
+  <si>
+    <t>donor_organism.medical_history.smoking_history</t>
+  </si>
+  <si>
+    <t>donor_organism.organism_age</t>
+  </si>
+  <si>
+    <t>donor_organism.organism_age_unit.text</t>
+  </si>
+  <si>
+    <t>donor_organism.organism_age_unit.ontology</t>
+  </si>
+  <si>
+    <t>donor_organism.development_stage.text</t>
+  </si>
+  <si>
+    <t>donor_organism.development_stage.ontology</t>
+  </si>
+  <si>
+    <t>donor_organism.disease.text</t>
+  </si>
+  <si>
+    <t>donor_organism.disease.ontology</t>
+  </si>
+  <si>
+    <t>donor_organism.height</t>
+  </si>
+  <si>
+    <t>donor_organism.height_unit.text</t>
+  </si>
+  <si>
+    <t>donor_organism.height_unit.ontology</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1401,13 +1395,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -1447,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1456,22 +1450,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -1538,7 +1532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1554,19 +1548,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="15" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,18 +1806,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1840,7 +1834,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1850,22 +1844,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="20" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -2103,91 +2097,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.5" style="4" customWidth="1"/>
-    <col min="2" max="3" width="30.33203125" style="4" customWidth="1"/>
-    <col min="4" max="20" width="30.33203125" style="4"/>
-    <col min="21" max="21" width="44.33203125" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="30.33203125" style="4"/>
+    <col min="1" max="1" width="61.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="58.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="45.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="30.33203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="11" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>174</v>
+        <v>250</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>175</v>
+        <v>251</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>176</v>
+        <v>252</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>177</v>
+        <v>253</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>178</v>
+        <v>254</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>179</v>
+        <v>255</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>180</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>181</v>
+        <v>257</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>182</v>
+        <v>258</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>183</v>
+        <v>259</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>184</v>
+        <v>260</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>185</v>
+        <v>261</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>186</v>
+        <v>262</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>187</v>
+        <v>263</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>191</v>
+        <v>267</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="X1" s="10" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -2330,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,46 +2365,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -2492,7 +2506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2508,31 +2522,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>235</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
@@ -2598,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2610,22 +2624,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -2675,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2688,22 +2702,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -2767,25 +2781,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -2851,49 +2865,49 @@
   <sheetData>
     <row r="1" spans="1:15" s="11" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added lookup for identifiable fields
</commit_message>
<xml_diff>
--- a/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
+++ b/tests/importer/data/HCA_metadata_Tissue_Stability_20180402_preview_release_new_headers.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/ingest-client/tests/importer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C67EC50E-DB13-4541-8843-E2B697FC1E61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1511F967-2C61-0D4D-B4EE-07F24D61BE4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="4700" windowWidth="32220" windowHeight="20480" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="4700" windowWidth="32220" windowHeight="20480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
     <sheet name="Contact" sheetId="3" r:id="rId2"/>
     <sheet name="Donor" sheetId="4" r:id="rId3"/>
     <sheet name="Specimen from organism" sheetId="6" r:id="rId4"/>
-    <sheet name="Cell suspension" sheetId="7" r:id="rId5"/>
-    <sheet name="Dissociation process" sheetId="12" r:id="rId6"/>
+    <sheet name="Dissociation process" sheetId="12" r:id="rId5"/>
+    <sheet name="Cell suspension" sheetId="7" r:id="rId6"/>
     <sheet name="Enrichment process" sheetId="13" r:id="rId7"/>
     <sheet name="Sequencing process" sheetId="15" r:id="rId8"/>
     <sheet name="Library preparation process" sheetId="14" r:id="rId9"/>
-    <sheet name="Protocols" sheetId="17" r:id="rId10"/>
-    <sheet name="Sequence files" sheetId="18" r:id="rId11"/>
+    <sheet name="Sequence files" sheetId="18" r:id="rId10"/>
+    <sheet name="Protocols" sheetId="17" r:id="rId11"/>
     <sheet name="schemas" sheetId="20" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="271">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>protocol.protocol_core.process_name</t>
+  </si>
+  <si>
+    <t>sequence_file.biomaterial_id</t>
   </si>
   <si>
     <t>sequence_file.lane_index</t>
@@ -1444,101 +1447,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="37.6640625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1554,19 +1466,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="15" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
@@ -1794,6 +1706,97 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="37.6640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2330,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2354,16 +2357,16 @@
         <v>209</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>192</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>224</v>
@@ -2476,6 +2479,50 @@
         <v>125</v>
       </c>
       <c r="N4" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="27">
+        <v>9606</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="27">
+        <v>7200</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="27">
+        <v>19800</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N5" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2489,116 +2536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="51" style="16" customWidth="1"/>
-    <col min="2" max="2" width="55.33203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" style="16"/>
-    <col min="4" max="4" width="50.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="78.5" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="32.1640625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="3">
-        <v>9606</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="17">
-        <v>39300000</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2625,7 +2566,7 @@
         <v>239</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -2668,6 +2609,112 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51" style="16" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="16"/>
+    <col min="4" max="4" width="32.1640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="78.5" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="32.1640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="3">
+        <v>9606</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="17">
+        <v>39300000</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2703,7 +2750,7 @@
         <v>243</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -2785,7 +2832,7 @@
         <v>254</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2940,7 @@
         <v>252</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="7" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>